<commit_message>
result parse tool done
</commit_message>
<xml_diff>
--- a/kcbp_cgal_cuda/Release/bunny Result.xlsx
+++ b/kcbp_cgal_cuda/Release/bunny Result.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="bunny2.k24.log.result" sheetId="1" r:id="rId1"/>
+    <sheet name="bunny" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>n</t>
   </si>
@@ -64,10 +64,6 @@
   </si>
   <si>
     <t>count(real)</t>
-  </si>
-  <si>
-    <t>kcbp 构造</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>对比</t>
@@ -104,12 +100,73 @@
   <si>
     <t>GJK traverse时间</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aabbBuildCount</t>
+  </si>
+  <si>
+    <t>模型数量n</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>按需构造kcbp时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>按需构造模型AABB时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kcbpModelCheckCount</t>
+  </si>
+  <si>
+    <t>kcbp构造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>KCBP碰撞检测时间(AABB)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>KCBP碰撞检测时间(GJK)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>之前的论文实验是碰撞的时候构造一次AABBTree. 没有复用构造好的AABBTree.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>init(kDOPTree)</t>
+  </si>
+  <si>
+    <t>CD(kDOPTree)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ConstructKCBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ConstructModelAABB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> init-CD(kCBP-aabb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> init-CD(kCBP-GJK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> count(kCBP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> count(real)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,8 +753,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1021,19 +1081,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1"/>
+    <col min="10" max="10" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1050,40 +1118,46 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1107,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1122,43 +1196,49 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O2">
         <v>2</v>
       </c>
       <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>30</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F12" si="0">SUM(B3:E3)</f>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G3">
         <v>130</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1173,75 +1253,87 @@
         <v>1</v>
       </c>
       <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>24</v>
+      </c>
+      <c r="O3">
         <v>42</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>31</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>31</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>50</v>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
         <v>6</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G4">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H4">
+        <v>46</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
+        <v>46</v>
+      </c>
+      <c r="O4">
         <v>66</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>43</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>43</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>70</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -1254,45 +1346,51 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G5">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
       <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="M5">
+      <c r="N5">
+        <v>68</v>
+      </c>
+      <c r="O5">
         <v>144</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>77</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>77</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>90</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1305,48 +1403,54 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G6">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
         <v>6</v>
       </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
       <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>88</v>
+      </c>
+      <c r="O6">
         <v>261</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>119</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>119</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -1356,40 +1460,46 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="G7">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
       <c r="J7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>7</v>
       </c>
       <c r="L7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>97</v>
+      </c>
+      <c r="O7">
         <v>335</v>
       </c>
-      <c r="N7">
-        <v>198</v>
-      </c>
-      <c r="O7">
+      <c r="P7">
         <v>200</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
+        <v>200</v>
+      </c>
+      <c r="R7">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>110</v>
       </c>
@@ -1397,7 +1507,7 @@
         <v>69</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>11</v>
@@ -1407,48 +1517,54 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G8">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
       <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
         <v>9</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>8</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>9</v>
       </c>
-      <c r="M8">
+      <c r="N8">
+        <v>108</v>
+      </c>
+      <c r="O8">
         <v>393</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>220</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>220</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>130</v>
       </c>
       <c r="B9">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>13</v>
@@ -1458,102 +1574,114 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G9">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="I9">
         <v>5</v>
       </c>
       <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>11</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="N9">
+        <v>130</v>
+      </c>
+      <c r="O9">
         <v>507</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>276</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>276</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>150</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>16</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G10">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="H10">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="I10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10">
         <v>15</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>16</v>
       </c>
-      <c r="L10">
-        <v>14</v>
-      </c>
       <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10">
+        <v>149</v>
+      </c>
+      <c r="O10">
         <v>727</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>423</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>424</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>170</v>
       </c>
       <c r="B11">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>13</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>18</v>
@@ -1563,51 +1691,57 @@
         <v>150</v>
       </c>
       <c r="G11">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
         <v>16</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>17</v>
       </c>
-      <c r="L11">
-        <v>16</v>
-      </c>
       <c r="M11">
+        <v>17</v>
+      </c>
+      <c r="N11">
+        <v>170</v>
+      </c>
+      <c r="O11">
         <v>786</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>431</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>431</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>328</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>200</v>
       </c>
       <c r="B12">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C12">
         <v>15</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1617,68 +1751,879 @@
         <v>1077</v>
       </c>
       <c r="H12">
+        <v>200</v>
+      </c>
+      <c r="I12">
+        <v>14</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>27</v>
+      </c>
+      <c r="L12">
+        <v>28</v>
+      </c>
+      <c r="M12">
+        <v>26</v>
+      </c>
+      <c r="N12">
+        <v>200</v>
+      </c>
+      <c r="O12">
+        <v>1328</v>
+      </c>
+      <c r="P12">
+        <v>718</v>
+      </c>
+      <c r="Q12">
+        <v>718</v>
+      </c>
+      <c r="R12">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="I12">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
+        <f>F2/A2*H2</f>
+        <v>2.7</v>
+      </c>
+      <c r="C26">
+        <f>G2/H2*N2</f>
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <f>J2+K2</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>L2+M2</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>282</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" ref="B27:B36" si="1">F3/A3*H3</f>
+        <v>25.6</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C36" si="2">G3/H3*N3</f>
+        <v>130</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:D36" si="3">J3+K3</f>
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27:E36" si="4">L3+M3</f>
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>2221</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>50</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="1"/>
+        <v>55.199999999999996</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>248</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>4280</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>70</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="1"/>
+        <v>58.285714285714285</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>368</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>6240</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="1"/>
+        <v>82.13333333333334</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>475</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>8073</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>100</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="1"/>
+        <v>100.88000000000001</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>526</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>8928</v>
+      </c>
+      <c r="G31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="1"/>
+        <v>99.163636363636371</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>581</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>9929</v>
+      </c>
+      <c r="G32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>130</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>699</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="F33">
+        <v>11962</v>
+      </c>
+      <c r="G33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>150</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="1"/>
+        <v>135.09333333333333</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>805</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="F34">
+        <v>13671</v>
+      </c>
+      <c r="G34">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>170</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>917.00000000000011</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <v>15599</v>
+      </c>
+      <c r="G35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>200</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="1"/>
+        <v>174</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>1077</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="F36">
+        <v>18525</v>
+      </c>
+      <c r="G36">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45">
         <v>9</v>
       </c>
-      <c r="J12">
-        <v>27</v>
-      </c>
-      <c r="K12">
+      <c r="C45">
+        <v>17</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46">
+        <v>32</v>
+      </c>
+      <c r="C46">
+        <v>130</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>31</v>
+      </c>
+      <c r="G46">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>248</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>43</v>
+      </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>70</v>
+      </c>
+      <c r="B48">
+        <v>60</v>
+      </c>
+      <c r="C48">
+        <v>368</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>77</v>
+      </c>
+      <c r="G48">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>90</v>
+      </c>
+      <c r="B49">
+        <v>84</v>
+      </c>
+      <c r="C49">
+        <v>475</v>
+      </c>
+      <c r="D49">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>119</v>
+      </c>
+      <c r="G49">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>100</v>
+      </c>
+      <c r="B50">
+        <v>104</v>
+      </c>
+      <c r="C50">
+        <v>526</v>
+      </c>
+      <c r="D50">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>200</v>
+      </c>
+      <c r="G50">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>110</v>
+      </c>
+      <c r="B51">
+        <v>101</v>
+      </c>
+      <c r="C51">
+        <v>581</v>
+      </c>
+      <c r="D51">
+        <v>14</v>
+      </c>
+      <c r="E51">
+        <v>17</v>
+      </c>
+      <c r="F51">
+        <v>220</v>
+      </c>
+      <c r="G51">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>130</v>
+      </c>
+      <c r="B52">
+        <v>109</v>
+      </c>
+      <c r="C52">
+        <v>699</v>
+      </c>
+      <c r="D52">
+        <v>16</v>
+      </c>
+      <c r="E52">
+        <v>21</v>
+      </c>
+      <c r="F52">
+        <v>276</v>
+      </c>
+      <c r="G52">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>150</v>
+      </c>
+      <c r="B53">
+        <v>136</v>
+      </c>
+      <c r="C53">
+        <v>805</v>
+      </c>
+      <c r="D53">
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>31</v>
+      </c>
+      <c r="F53">
+        <v>423</v>
+      </c>
+      <c r="G53">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>170</v>
+      </c>
+      <c r="B54">
+        <v>150</v>
+      </c>
+      <c r="C54">
+        <v>917</v>
+      </c>
+      <c r="D54">
+        <v>24</v>
+      </c>
+      <c r="E54">
+        <v>34</v>
+      </c>
+      <c r="F54">
+        <v>431</v>
+      </c>
+      <c r="G54">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>200</v>
+      </c>
+      <c r="B55">
+        <v>174</v>
+      </c>
+      <c r="C55">
+        <v>1077</v>
+      </c>
+      <c r="D55">
+        <v>35</v>
+      </c>
+      <c r="E55">
+        <v>54</v>
+      </c>
+      <c r="F55">
+        <v>718</v>
+      </c>
+      <c r="G55">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>282</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <v>2221</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>42</v>
+      </c>
+      <c r="G64">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65">
+        <v>4280</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>66</v>
+      </c>
+      <c r="G65">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C66">
+        <v>70</v>
+      </c>
+      <c r="D66">
+        <v>6240</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>144</v>
+      </c>
+      <c r="G66">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C67">
+        <v>90</v>
+      </c>
+      <c r="D67">
+        <v>8073</v>
+      </c>
+      <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
+        <v>261</v>
+      </c>
+      <c r="G67">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C68">
+        <v>100</v>
+      </c>
+      <c r="D68">
+        <v>8928</v>
+      </c>
+      <c r="E68">
+        <v>13</v>
+      </c>
+      <c r="F68">
+        <v>335</v>
+      </c>
+      <c r="G68">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C69">
+        <v>110</v>
+      </c>
+      <c r="D69">
+        <v>9929</v>
+      </c>
+      <c r="E69">
+        <v>13</v>
+      </c>
+      <c r="F69">
+        <v>393</v>
+      </c>
+      <c r="G69">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C70">
+        <v>130</v>
+      </c>
+      <c r="D70">
+        <v>11962</v>
+      </c>
+      <c r="E70">
+        <v>17</v>
+      </c>
+      <c r="F70">
+        <v>507</v>
+      </c>
+      <c r="G70">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C71">
+        <v>150</v>
+      </c>
+      <c r="D71">
+        <v>13671</v>
+      </c>
+      <c r="E71">
         <v>28</v>
       </c>
-      <c r="L12">
-        <v>26</v>
-      </c>
-      <c r="M12">
+      <c r="F71">
+        <v>727</v>
+      </c>
+      <c r="G71">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C72">
+        <v>170</v>
+      </c>
+      <c r="D72">
+        <v>15599</v>
+      </c>
+      <c r="E72">
+        <v>29</v>
+      </c>
+      <c r="F72">
+        <v>786</v>
+      </c>
+      <c r="G72">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.15">
+      <c r="C73">
+        <v>200</v>
+      </c>
+      <c r="D73">
+        <v>18525</v>
+      </c>
+      <c r="E73">
+        <v>49</v>
+      </c>
+      <c r="F73">
         <v>1328</v>
       </c>
-      <c r="N12">
-        <v>718</v>
-      </c>
-      <c r="O12">
-        <v>718</v>
-      </c>
-      <c r="P12">
+      <c r="G73">
         <v>556</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="F23" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>